<commit_message>
validación de carga y backup proceso de carga del ETL
</commit_message>
<xml_diff>
--- a/data/input/exhibiciones/exhibiciones.xlsx
+++ b/data/input/exhibiciones/exhibiciones.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\desarrollo\gestionCompras\data\input\exhibiciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B194EAE-3E0E-4059-B3C4-CE609E69ED94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E47C0407-5818-4E1A-BACB-E2869EEBA150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -378,7 +378,7 @@
   <dimension ref="A1:E187"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>